<commit_message>
add taiwind css for framework stayle
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="7">
   <si>
     <t>Data</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>Design Card Css</t>
   </si>
 </sst>
 </file>
@@ -94,11 +97,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,24 +384,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G2"/>
+  <dimension ref="B2:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.21875" defaultRowHeight="32.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.21875" defaultRowHeight="32.4" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" customWidth="1"/>
-    <col min="6" max="6" width="37" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="42" style="2" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="13.21875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,6 +420,14 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="3">
+        <v>44256</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>